<commit_message>
clean up and comment code
</commit_message>
<xml_diff>
--- a/machine_learning/data/machine_learning/template_linearized.xlsx
+++ b/machine_learning/data/machine_learning/template_linearized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinsse/Documents/github/biodefluorination-paper/machine_learning/data/machine_learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688AE1DF-71D4-0349-9787-1E80B75BC54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7207D80E-9A40-1E4F-BE0A-F03145C6EC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10940" yWindow="500" windowWidth="26040" windowHeight="13580" xr2:uid="{4C67F7C5-C32F-6B40-94D5-DA22915FCE92}"/>
+    <workbookView xWindow="2340" yWindow="2840" windowWidth="26040" windowHeight="13580" xr2:uid="{4C67F7C5-C32F-6B40-94D5-DA22915FCE92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -802,7 +802,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -812,6 +812,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC9E0F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,12 +850,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1167,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC1971C-B515-5A46-9FB2-DB5CAF6D50A8}">
   <dimension ref="A1:AM22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1553,98 +1564,98 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Y5" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AA5" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AB5" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AC5" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AD5" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="AE5" s="2" t="s">
+      <c r="AE5" s="4" t="s">
         <v>224</v>
       </c>
     </row>

</xml_diff>